<commit_message>
Spring Security RememberMe トークンの保存に DB を使用
</commit_message>
<xml_diff>
--- a/java/spring-security/doc/remember-me.xlsx
+++ b/java/spring-security/doc/remember-me.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="1155" windowWidth="15105" windowHeight="8655" activeTab="2"/>
+    <workbookView xWindow="720" yWindow="1155" windowWidth="15105" windowHeight="8655" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="58">
   <si>
     <t>PersistentRememberMeToken</t>
     <phoneticPr fontId="1"/>
@@ -138,14 +138,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>series0-token1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>series0-token0</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>トークン</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -157,13 +149,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>トークンを発行</t>
-    <rPh sb="5" eb="7">
-      <t>ハッコウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>トークンを保存</t>
     <rPh sb="5" eb="7">
       <t>ホゾン</t>
@@ -182,13 +167,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>トークンを更新</t>
-    <rPh sb="5" eb="7">
-      <t>コウシン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>セッション切れ</t>
     <rPh sb="5" eb="6">
       <t>ギ</t>
@@ -196,24 +174,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>再アクセス</t>
-    <rPh sb="0" eb="1">
-      <t>サイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>保存されているトークンと
-異なるのでエラー</t>
-    <rPh sb="0" eb="2">
-      <t>ホゾン</t>
-    </rPh>
-    <rPh sb="13" eb="14">
-      <t>コト</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>トークンを生成</t>
     <rPh sb="5" eb="7">
       <t>セイセイ</t>
@@ -226,6 +186,304 @@
   </si>
   <si>
     <t>token3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Cookie を発行</t>
+    <rPh sb="8" eb="10">
+      <t>ハッコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Cookie</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>シリーズ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>シリーズとトークンの組み合わせを記録</t>
+    <rPh sb="10" eb="11">
+      <t>ク</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>キロク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Series1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Token1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>Series１</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>Token１</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Cookie からシリーズを取得</t>
+    <rPh sb="14" eb="16">
+      <t>シュトク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Cookie のトークンとサーバーが記録していたトークンが一致するか検証</t>
+    <rPh sb="18" eb="20">
+      <t>キロク</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>イッチ</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>ケンショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>サーバーの記録</t>
+    <rPh sb="5" eb="7">
+      <t>キロク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>シリーズでサーバーの記録を検索してトークンを取得</t>
+    <rPh sb="10" eb="12">
+      <t>キロク</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>シュトク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Token2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>一致する場合は自動ログインを行い、新しいトークンを生成して Cookie の値を更新する</t>
+    <rPh sb="0" eb="2">
+      <t>イッチ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ジドウ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>アタラ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>セイセイ</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>アタイ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>コウシン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>一致しない場合は</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve"> Cookie が盗まれた可能性があると判断して、エラーにする</t>
+    </r>
+    <rPh sb="0" eb="2">
+      <t>イッチ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>ヌス</t>
+    </rPh>
+    <rPh sb="21" eb="24">
+      <t>カノウセイ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>ハンダン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>Series１</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>Token2</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Cookie を更新</t>
+    <rPh sb="8" eb="10">
+      <t>コウシン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>エラーになる</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>サーバーが記録しているトークン（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>Token2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>）が一致しないので</t>
+    </r>
+    <rPh sb="5" eb="7">
+      <t>キロク</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>イッチ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>Series１</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>Token１</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>Cookie のトークン（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>Token1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>）と</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>被害者</t>
+    <rPh sb="0" eb="3">
+      <t>ヒガイシャ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -233,7 +491,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,16 +528,69 @@
       <family val="3"/>
       <charset val="128"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="メイリオ"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="メイリオ"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="メイリオ"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="メイリオ"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="メイリオ"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="メイリオ"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -287,19 +598,97 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -318,16 +707,1553 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>408365</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>156882</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="直線コネクタ 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3190875" y="514350"/>
+          <a:ext cx="0" cy="3143250"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="直線コネクタ 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6981825" y="514350"/>
+          <a:ext cx="0" cy="2838450"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="直線矢印コネクタ 5"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="923925" y="1000125"/>
+          <a:ext cx="3400425" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>57151</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>627530</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>235323</xdr:rowOff>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="テキスト ボックス 6"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1943101" y="552450"/>
+          <a:ext cx="1143000" cy="390525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:latin typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>ログイン</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="直線矢印コネクタ 7"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="923925" y="2714625"/>
+          <a:ext cx="3400425" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="曲線コネクタ 10"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2552700" y="3352800"/>
+          <a:ext cx="4895850" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="曲線コネクタ 11"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2552700" y="3533775"/>
+          <a:ext cx="4895850" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="直線コネクタ 14"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6981825" y="3552825"/>
+          <a:ext cx="0" cy="3886200"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="直線コネクタ 15"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3190875" y="3857625"/>
+          <a:ext cx="0" cy="3629025"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="テキスト ボックス 16"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1200150" y="3571875"/>
+          <a:ext cx="1228726" cy="390525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:latin typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>セッション切れ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="直線矢印コネクタ 17"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3324225" y="4448175"/>
+          <a:ext cx="3400425" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>57151</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="テキスト ボックス 18"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4343401" y="4048125"/>
+          <a:ext cx="1143000" cy="390525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:latin typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>アクセス</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="直線矢印コネクタ 19"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3324225" y="7067550"/>
+          <a:ext cx="3400425" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="直線コネクタ 22"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3190875" y="9324975"/>
+          <a:ext cx="0" cy="4610100"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="直線コネクタ 23"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6981825" y="9324975"/>
+          <a:ext cx="0" cy="7296150"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="直線矢印コネクタ 24"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3324225" y="1000125"/>
+          <a:ext cx="3400425" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>57151</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="テキスト ボックス 25"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4343401" y="552450"/>
+          <a:ext cx="1143000" cy="390525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:latin typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>ログイン</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="直線矢印コネクタ 26"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3324225" y="2714625"/>
+          <a:ext cx="3400425" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>14454</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="曲線コネクタ 27"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2381250" y="13825704"/>
+          <a:ext cx="1885950" cy="128422"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>142876</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="テキスト ボックス 31"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1143000" y="13849350"/>
+          <a:ext cx="1228726" cy="390525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:latin typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>セッション切れ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>67</xdr:col>
+      <xdr:colOff>85726</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="直線矢印コネクタ 32"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7105650" y="13258800"/>
+          <a:ext cx="4467226" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>142876</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>58</xdr:col>
+      <xdr:colOff>85726</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="テキスト ボックス 33"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8886826" y="12915900"/>
+          <a:ext cx="1143000" cy="390525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:latin typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>アクセス</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>68</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>68</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="直線コネクタ 35"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11744325" y="9324975"/>
+          <a:ext cx="0" cy="6686550"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>67</xdr:col>
+      <xdr:colOff>104776</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="直線矢印コネクタ 36"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3343275" y="12182475"/>
+          <a:ext cx="8248651" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>57151</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="テキスト ボックス 39"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4343401" y="11849100"/>
+          <a:ext cx="1476374" cy="390525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:latin typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>Cookie </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:latin typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>を盗む</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>166854</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="48" name="曲線コネクタ 47"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2381250" y="13978104"/>
+          <a:ext cx="1885950" cy="128422"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="50" name="直線コネクタ 49"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3190875" y="14087475"/>
+          <a:ext cx="0" cy="2543175"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="52" name="直線矢印コネクタ 51"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3324225" y="16278225"/>
+          <a:ext cx="3514725" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>57151</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="53" name="テキスト ボックス 52"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4514851" y="15849600"/>
+          <a:ext cx="1143000" cy="390525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:latin typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="メイリオ" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>アクセス</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>67</xdr:col>
+      <xdr:colOff>104777</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="56" name="直線矢印コネクタ 55"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7143750" y="15554325"/>
+          <a:ext cx="4448177" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>151190</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>4482</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>313205</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>82923</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -336,7 +2262,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="12124115" y="633132"/>
+          <a:off x="836990" y="4052607"/>
           <a:ext cx="11191965" cy="1507191"/>
           <a:chOff x="329923" y="1613647"/>
           <a:chExt cx="11156106" cy="1490382"/>
@@ -1383,135 +3309,379 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G13"/>
+  <dimension ref="H2:BS70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="CK45" sqref="CK45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="2.25" defaultRowHeight="18.75" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="1"/>
+    <col min="1" max="16384" width="2.25" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="8:52" x14ac:dyDescent="0.45">
+      <c r="Q2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="AN2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="1" t="s">
+    </row>
+    <row r="5" spans="8:52" x14ac:dyDescent="0.45">
+      <c r="AQ5" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="8:52" x14ac:dyDescent="0.45">
+      <c r="AQ6" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="8:52" x14ac:dyDescent="0.45">
+      <c r="AQ7" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="8:52" x14ac:dyDescent="0.45">
+      <c r="AQ8" s="12"/>
+    </row>
+    <row r="9" spans="8:52" x14ac:dyDescent="0.45">
+      <c r="AQ9" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="8:52" x14ac:dyDescent="0.45">
+      <c r="AQ10" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="8:52" x14ac:dyDescent="0.45">
+      <c r="H11" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ11" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="AR11" s="15"/>
+      <c r="AS11" s="10"/>
+      <c r="AT11" s="10"/>
+      <c r="AU11" s="11"/>
+      <c r="AV11" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW11" s="10"/>
+      <c r="AX11" s="10"/>
+      <c r="AY11" s="10"/>
+      <c r="AZ11" s="11"/>
+    </row>
+    <row r="12" spans="8:52" x14ac:dyDescent="0.45">
+      <c r="H12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ12" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="AR12" s="7"/>
+      <c r="AS12" s="7"/>
+      <c r="AT12" s="7"/>
+      <c r="AU12" s="8"/>
+      <c r="AV12" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="AW12" s="7"/>
+      <c r="AX12" s="7"/>
+      <c r="AY12" s="7"/>
+      <c r="AZ12" s="8"/>
+    </row>
+    <row r="18" spans="8:52" x14ac:dyDescent="0.45">
+      <c r="H18" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="8:52" x14ac:dyDescent="0.45">
+      <c r="H19" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ19" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="8:52" x14ac:dyDescent="0.45">
+      <c r="AQ20" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="8:52" x14ac:dyDescent="0.45">
+      <c r="AQ22" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="8:52" x14ac:dyDescent="0.45">
+      <c r="AQ24" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="8:52" x14ac:dyDescent="0.45">
+      <c r="AQ25" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="8:52" x14ac:dyDescent="0.45">
+      <c r="AQ27" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="8:52" x14ac:dyDescent="0.45">
+      <c r="AQ28" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="8:52" x14ac:dyDescent="0.45">
+      <c r="Z29" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AQ29" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="8:52" x14ac:dyDescent="0.45">
+      <c r="H30" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AQ30" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="AR30" s="10"/>
+      <c r="AS30" s="10"/>
+      <c r="AT30" s="10"/>
+      <c r="AU30" s="11"/>
+      <c r="AV30" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW30" s="10"/>
+      <c r="AX30" s="10"/>
+      <c r="AY30" s="10"/>
+      <c r="AZ30" s="11"/>
+    </row>
+    <row r="31" spans="8:52" x14ac:dyDescent="0.45">
+      <c r="H31" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AQ31" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="AR31" s="7"/>
+      <c r="AS31" s="7"/>
+      <c r="AT31" s="7"/>
+      <c r="AU31" s="8"/>
+      <c r="AV31" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="AW31" s="7"/>
+      <c r="AX31" s="7"/>
+      <c r="AY31" s="7"/>
+      <c r="AZ31" s="8"/>
+    </row>
+    <row r="39" spans="8:68" x14ac:dyDescent="0.45">
+      <c r="R39" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN39" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="BP39" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="D5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="F7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="F8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="D9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="1" t="s">
+    <row r="42" spans="8:68" x14ac:dyDescent="0.45">
+      <c r="AQ42" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="8:68" x14ac:dyDescent="0.45">
+      <c r="AQ43" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="8:68" x14ac:dyDescent="0.45">
+      <c r="AQ44" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="8:68" x14ac:dyDescent="0.45">
+      <c r="AQ45" s="12"/>
+    </row>
+    <row r="46" spans="8:68" x14ac:dyDescent="0.45">
+      <c r="AQ46" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="8:68" x14ac:dyDescent="0.45">
+      <c r="AQ47" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="8:68" x14ac:dyDescent="0.45">
+      <c r="H48" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z48" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ48" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="AR48" s="15"/>
+      <c r="AS48" s="10"/>
+      <c r="AT48" s="10"/>
+      <c r="AU48" s="11"/>
+      <c r="AV48" s="10" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="F10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="AW48" s="10"/>
+      <c r="AX48" s="10"/>
+      <c r="AY48" s="10"/>
+      <c r="AZ48" s="11"/>
+    </row>
+    <row r="49" spans="8:71" x14ac:dyDescent="0.45">
+      <c r="H49" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ49" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="AR49" s="7"/>
+      <c r="AS49" s="7"/>
+      <c r="AT49" s="7"/>
+      <c r="AU49" s="8"/>
+      <c r="AV49" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="AW49" s="7"/>
+      <c r="AX49" s="7"/>
+      <c r="AY49" s="7"/>
+      <c r="AZ49" s="8"/>
+    </row>
+    <row r="51" spans="8:71" x14ac:dyDescent="0.45">
+      <c r="BS51" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="8:71" x14ac:dyDescent="0.45">
+      <c r="BS52" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="55" spans="8:71" x14ac:dyDescent="0.45">
+      <c r="H55" s="12"/>
+    </row>
+    <row r="56" spans="8:71" x14ac:dyDescent="0.45">
+      <c r="H56" s="6"/>
+      <c r="BS56" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="57" spans="8:71" x14ac:dyDescent="0.45">
+      <c r="BS57" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="58" spans="8:71" x14ac:dyDescent="0.45">
+      <c r="AQ58" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="59" spans="8:71" x14ac:dyDescent="0.45">
+      <c r="AQ59" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="60" spans="8:71" x14ac:dyDescent="0.45">
+      <c r="AQ60" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="61" spans="8:71" x14ac:dyDescent="0.45">
+      <c r="AQ61" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="62" spans="8:71" x14ac:dyDescent="0.45">
+      <c r="AQ62" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="AR62" s="10"/>
+      <c r="AS62" s="10"/>
+      <c r="AT62" s="10"/>
+      <c r="AU62" s="11"/>
+      <c r="AV62" s="10" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B12" s="1" t="s">
+      <c r="AW62" s="10"/>
+      <c r="AX62" s="10"/>
+      <c r="AY62" s="10"/>
+      <c r="AZ62" s="11"/>
+    </row>
+    <row r="63" spans="8:71" x14ac:dyDescent="0.45">
+      <c r="AQ63" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="AR63" s="7"/>
+      <c r="AS63" s="7"/>
+      <c r="AT63" s="7"/>
+      <c r="AU63" s="8"/>
+      <c r="AV63" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="AW63" s="7"/>
+      <c r="AX63" s="7"/>
+      <c r="AY63" s="7"/>
+      <c r="AZ63" s="8"/>
+    </row>
+    <row r="65" spans="8:71" x14ac:dyDescent="0.45">
+      <c r="AZ65" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="BS65" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="37.5" x14ac:dyDescent="0.45">
-      <c r="D13" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>28</v>
+    </row>
+    <row r="66" spans="8:71" x14ac:dyDescent="0.45">
+      <c r="Z66" s="6"/>
+      <c r="BS66" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="68" spans="8:71" x14ac:dyDescent="0.45">
+      <c r="H68" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AQ68" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="69" spans="8:71" x14ac:dyDescent="0.45">
+      <c r="H69" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AQ69" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="70" spans="8:71" x14ac:dyDescent="0.45">
+      <c r="AQ70" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1519,8 +3689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.45"/>
@@ -1548,22 +3718,22 @@
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.45">
@@ -1573,7 +3743,7 @@
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.45">
       <c r="D5" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>27</v>
@@ -1581,7 +3751,7 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>27</v>
@@ -1589,7 +3759,7 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.45">
       <c r="F7" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>27</v>
@@ -1597,7 +3767,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.45">
       <c r="F8" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>27</v>
@@ -1605,23 +3775,23 @@
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.45">
       <c r="D9" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.45">
       <c r="F10" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>27</v>
@@ -1629,7 +3799,7 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>27</v>
@@ -1637,10 +3807,10 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.45">
       <c r="D13" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="6:17" x14ac:dyDescent="0.45">

</xml_diff>